<commit_message>
modified PGP treatment to allow different to and from technologies
</commit_message>
<xml_diff>
--- a/case_input_test_PGP_wind_solar.xlsx
+++ b/case_input_test_PGP_wind_solar.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20228"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{470B7A58-8FD0-4BFC-873F-C8715FA2989B}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9340FB70-9A33-4052-A02C-13577F012D46}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15500" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="110" uniqueCount="97">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="102">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -172,9 +172,6 @@
     <t>CAPACITY_COST_WIND</t>
   </si>
   <si>
-    <t>$/kWh</t>
-  </si>
-  <si>
     <t>DISPATCH_COST_WIND</t>
   </si>
   <si>
@@ -280,18 +277,9 @@
     <t>PGP_STORAGE_CHARGING_EFFICIENCY</t>
   </si>
   <si>
-    <t>CAPACITY_COST_PGP_FUEL_CELL</t>
-  </si>
-  <si>
     <t>1e-6 adds on about 1 cent per kWh if used one cycle per year</t>
   </si>
   <si>
-    <t>This will add 1 cent per h per kW capacity</t>
-  </si>
-  <si>
-    <t>0.01 means 1 cent per hour per kW capacity</t>
-  </si>
-  <si>
     <t>($/h)/kW</t>
   </si>
   <si>
@@ -311,6 +299,33 @@
   </si>
   <si>
     <t>battery03</t>
+  </si>
+  <si>
+    <t>QUICK_LOOK</t>
+  </si>
+  <si>
+    <t>New "quick look" postprocessing.</t>
+  </si>
+  <si>
+    <t>CAPACITY_COST_TO_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t>CAPACITY_COST_FROM_PGP_STORAGE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrolyser $1100 per kW capital cost. Assume 10% capital recovery factor and 10,000 hours per year = </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrolyser $4600 per kW capital cost. Assume 10% capital recovery factor and 10,000 hours per year = </t>
+  </si>
+  <si>
+    <t>($/h)/kWh</t>
+  </si>
+  <si>
+    <t>If we assume $261/kWh capacity with a 10% cap recovery factor and 10,000 hours per year (and 6 hour charge/discharge time)</t>
+  </si>
+  <si>
+    <t>from $1568/kW and $261/kWh from Davis et al 2018</t>
   </si>
 </sst>
 </file>
@@ -1202,10 +1217,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F104"/>
+  <dimension ref="A1:F106"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="B93" sqref="B93"/>
+    <sheetView tabSelected="1" topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="E93" sqref="E93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1393,7 +1408,7 @@
         <v>22</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>23</v>
@@ -1438,96 +1453,97 @@
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A44" s="5"/>
-      <c r="B44" s="12"/>
-      <c r="C44" s="2"/>
+      <c r="A44" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="B44" s="12" t="b">
+        <v>1</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A45" s="5" t="s">
-        <v>31</v>
-      </c>
-      <c r="B45" s="12" t="s">
-        <v>77</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>32</v>
-      </c>
+      <c r="A45" s="5"/>
+      <c r="B45" s="12"/>
+      <c r="C45" s="2"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="13">
-        <v>1000000000</v>
+        <v>31</v>
+      </c>
+      <c r="B46" s="12" t="s">
+        <v>76</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>74</v>
+        <v>32</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B47" s="13">
         <v>1000000000</v>
       </c>
       <c r="C47" s="2" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="C48" s="2"/>
-    </row>
-    <row r="49" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A49" s="3" t="s">
+      <c r="A48" s="5" t="s">
+        <v>72</v>
+      </c>
+      <c r="B48" s="13">
+        <v>1000000000</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="C49" s="2"/>
+    </row>
+    <row r="50" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B49" s="11" t="s">
+      <c r="B50" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="C49" s="4"/>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C50" s="2"/>
+      <c r="C50" s="4"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A51" s="5" t="s">
+      <c r="C51" s="2"/>
+    </row>
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A52" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="B51" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="C51" s="2"/>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A52" s="5"/>
-      <c r="B52" s="12"/>
+      <c r="B52" s="12" t="s">
+        <v>79</v>
+      </c>
       <c r="C52" s="2"/>
-      <c r="D52" s="2"/>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A53" s="5" t="s">
-        <v>36</v>
-      </c>
-      <c r="B53" s="12">
-        <v>2006</v>
-      </c>
+      <c r="A53" s="5"/>
+      <c r="B53" s="12"/>
       <c r="C53" s="2"/>
       <c r="D53" s="2"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B54" s="12">
-        <v>1</v>
+        <v>2006</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B55" s="12">
         <v>1</v>
@@ -1537,7 +1553,7 @@
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B56" s="12">
         <v>1</v>
@@ -1547,429 +1563,455 @@
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B57" s="12">
-        <v>2006</v>
+        <v>1</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B58" s="12">
-        <v>12</v>
+        <v>2006</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B59" s="12">
-        <v>31</v>
+        <v>12</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B60" s="12">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A61" s="5"/>
-      <c r="B61" s="12"/>
+      <c r="A61" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B61" s="12">
+        <v>24</v>
+      </c>
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A62" s="5" t="s">
-        <v>44</v>
-      </c>
-      <c r="B62" s="12" t="s">
-        <v>78</v>
-      </c>
+      <c r="A62" s="5"/>
+      <c r="B62" s="12"/>
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B63" s="12">
-        <v>2.5000000000000001E-2</v>
-      </c>
-      <c r="C63" s="2" t="s">
-        <v>90</v>
-      </c>
+        <v>44</v>
+      </c>
+      <c r="B63" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
+        <v>45</v>
+      </c>
+      <c r="B64" s="12">
+        <v>2.5000000000000001E-2</v>
+      </c>
+      <c r="C64" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D64" s="2"/>
+    </row>
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A65" s="5" t="s">
         <v>46</v>
       </c>
-      <c r="B64" s="12">
+      <c r="B65" s="12">
         <f>0.00000001</f>
         <v>1E-8</v>
       </c>
-      <c r="C64" s="2" t="s">
+      <c r="C65" s="2" t="s">
         <v>47</v>
       </c>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A65" s="5"/>
-      <c r="B65" s="12"/>
-      <c r="C65" s="2"/>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A66" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B66" s="12" t="s">
-        <v>79</v>
-      </c>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A66" s="5"/>
+      <c r="B66" s="12"/>
       <c r="C66" s="2"/>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B67" s="12" t="s">
+        <v>78</v>
+      </c>
+      <c r="C67" s="2"/>
+      <c r="D67" s="2"/>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A68" s="5" t="s">
         <v>49</v>
       </c>
-      <c r="B67" s="12">
+      <c r="B68" s="12">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="C67" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A68" s="5" t="s">
+      <c r="C68" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D68" s="2"/>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A69" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" s="13">
+        <v>1E-8</v>
+      </c>
+      <c r="C69" s="2" t="s">
         <v>51</v>
       </c>
-      <c r="B68" s="13">
-        <v>1E-8</v>
-      </c>
-      <c r="C68" s="2" t="s">
+      <c r="D69" s="2"/>
+    </row>
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A70" s="5"/>
+      <c r="B70" s="12"/>
+      <c r="C70" s="2"/>
+      <c r="D70" s="2"/>
+    </row>
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A71" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A69" s="5"/>
-      <c r="B69" s="12"/>
-      <c r="C69" s="2"/>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A70" s="5" t="s">
+      <c r="B71" s="12">
+        <v>-1</v>
+      </c>
+      <c r="C71" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D71" s="2" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A72" s="5" t="s">
         <v>53</v>
       </c>
-      <c r="B70" s="12">
-        <v>-1</v>
-      </c>
-      <c r="C70" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D70" s="2" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A71" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="B71" s="12">
+      <c r="B72" s="12">
         <f>0.023</f>
         <v>2.3E-2</v>
       </c>
-      <c r="C71" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A72" s="5"/>
-      <c r="B72" s="12"/>
-      <c r="C72" s="2"/>
+      <c r="C72" s="2" t="s">
+        <v>86</v>
+      </c>
       <c r="D72" s="2"/>
     </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A73" s="5" t="s">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A73" s="5"/>
+      <c r="B73" s="12"/>
+      <c r="C73" s="2"/>
+      <c r="D73" s="2"/>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A74" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B74" s="12">
+        <v>-1</v>
+      </c>
+      <c r="C74" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D74" s="2" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A75" s="5" t="s">
         <v>55</v>
       </c>
-      <c r="B73" s="12">
-        <v>-1</v>
-      </c>
-      <c r="C73" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D73" s="2" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A74" s="5" t="s">
+      <c r="B75" s="12">
+        <v>1E-3</v>
+      </c>
+      <c r="C75" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D75" s="2"/>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A76" s="5"/>
+      <c r="B76" s="12"/>
+      <c r="C76" s="2"/>
+      <c r="D76" s="2"/>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A77" s="5" t="s">
         <v>56</v>
       </c>
-      <c r="B74" s="12">
-        <v>1E-3</v>
-      </c>
-      <c r="C74" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A75" s="5"/>
-      <c r="B75" s="12"/>
-      <c r="C75" s="2"/>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A76" s="5" t="s">
+      <c r="B77" s="12">
+        <v>2.6099999999999999E-3</v>
+      </c>
+      <c r="C77" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D77" s="2" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A78" s="5" t="s">
         <v>57</v>
-      </c>
-      <c r="B76" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="C76" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D76" s="2" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A77" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B77" s="12">
-        <v>0</v>
-      </c>
-      <c r="C77" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A78" s="5" t="s">
-        <v>59</v>
       </c>
       <c r="B78" s="12">
         <v>0</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>50</v>
+        <v>86</v>
       </c>
       <c r="D78" s="2"/>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B79" s="12">
+        <v>0</v>
+      </c>
+      <c r="C79" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D79" s="2"/>
+    </row>
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A80" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B80" s="12">
+        <v>0.9</v>
+      </c>
+      <c r="C80" s="2"/>
+      <c r="D80" s="2"/>
+    </row>
+    <row r="81" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A81" s="5" t="s">
         <v>60</v>
       </c>
-      <c r="B79" s="12">
-        <v>0.9</v>
-      </c>
-      <c r="C79" s="2"/>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
-      <c r="A80" s="5" t="s">
+      <c r="B81" s="12">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="C81" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="B80" s="12">
-        <v>1.0000000000000001E-5</v>
-      </c>
-      <c r="C80" s="2" t="s">
+      <c r="D81" s="2"/>
+      <c r="E81" s="1">
+        <v>7.3048000000000002E-3</v>
+      </c>
+      <c r="F81" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="D80" s="2"/>
-      <c r="E80" s="1">
-        <v>7.3048000000000002E-3</v>
-      </c>
-      <c r="F80" s="1" t="s">
+    </row>
+    <row r="82" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A82" s="5" t="s">
         <v>63</v>
       </c>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A81" s="5" t="s">
+      <c r="B82" s="12">
+        <v>6</v>
+      </c>
+      <c r="C82" s="2" t="s">
         <v>64</v>
       </c>
-      <c r="B81" s="12">
-        <v>4</v>
-      </c>
-      <c r="C81" s="2" t="s">
+      <c r="D82" s="2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A83" s="5"/>
+      <c r="B83" s="12"/>
+      <c r="C83" s="2"/>
+      <c r="D83" s="2"/>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A84" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="B84" s="12">
+        <v>9.9999999999999995E-7</v>
+      </c>
+      <c r="C84" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D84" s="2" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A85" s="5" t="s">
+        <v>95</v>
+      </c>
+      <c r="B85" s="12">
+        <v>1.0999999999999999E-2</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A86" s="5" t="s">
+        <v>96</v>
+      </c>
+      <c r="B86" s="12">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A87" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="B87" s="12">
+        <v>0</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D87" s="2"/>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A88" s="5" t="s">
+        <v>83</v>
+      </c>
+      <c r="B88" s="12">
+        <v>0</v>
+      </c>
+      <c r="C88" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="D88" s="2"/>
+    </row>
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A89" s="5" t="s">
+        <v>84</v>
+      </c>
+      <c r="B89" s="12">
+        <v>0.3</v>
+      </c>
+      <c r="C89" s="2"/>
+      <c r="D89" s="2"/>
+    </row>
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A90" s="5"/>
+      <c r="B90" s="12"/>
+      <c r="C90" s="2"/>
+      <c r="D90" s="2"/>
+    </row>
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A91" s="5" t="s">
         <v>65</v>
       </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A82" s="5"/>
-      <c r="B82" s="12"/>
-      <c r="C82" s="2"/>
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A83" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="B83" s="12">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="C83" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D83" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A84" s="5" t="s">
+      <c r="B91" s="12">
+        <v>10</v>
+      </c>
+      <c r="C91" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="B84" s="12">
-        <v>0.01</v>
-      </c>
-      <c r="C84" s="2" t="s">
-        <v>90</v>
-      </c>
-      <c r="D84" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A85" s="5" t="s">
-        <v>83</v>
-      </c>
-      <c r="B85" s="12">
-        <v>0</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A86" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="B86" s="12">
-        <v>0</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
-        <v>85</v>
-      </c>
-      <c r="B87" s="12">
-        <v>0.3</v>
-      </c>
-      <c r="C87" s="2"/>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A88" s="5"/>
-      <c r="B88" s="12"/>
-      <c r="C88" s="2"/>
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A89" s="5" t="s">
+      <c r="D91" s="2"/>
+    </row>
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="C93" s="2" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="94" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A94" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B89" s="12">
-        <v>10</v>
-      </c>
-      <c r="C89" s="2" t="s">
-        <v>50</v>
-      </c>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C90" s="2"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="C91" s="2" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="92" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A92" s="3" t="s">
+      <c r="B94" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="B92" s="11" t="s">
+      <c r="C94" s="4"/>
+    </row>
+    <row r="95" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A95" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="C92" s="4"/>
-    </row>
-    <row r="93" spans="1:4" s="5" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A93" s="5" t="s">
-        <v>69</v>
-      </c>
-      <c r="B93" s="5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="B94" s="1"/>
-    </row>
-    <row r="95" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A95" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="B95" s="8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="96" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A96" s="8" t="s">
-        <v>96</v>
-      </c>
-      <c r="B96" s="8">
-        <v>3.0000000000000001E-3</v>
-      </c>
+      <c r="B95" s="5" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="B96" s="1"/>
     </row>
     <row r="97" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A97" s="8" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B97" s="8">
-        <v>1E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="B98" s="8">
+        <v>3.0000000000000001E-3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A99" s="8" t="s">
+        <v>89</v>
+      </c>
+      <c r="B99" s="8">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A100" s="8" t="s">
+        <v>90</v>
+      </c>
+      <c r="B100" s="8">
         <v>2.9999999999999997E-4</v>
       </c>
     </row>
-    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="3" t="s">
+    <row r="102" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A102" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B102" s="11"/>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A106" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="B100" s="11"/>
-    </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A104" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated PGP_wind_solar case input file
</commit_message>
<xml_diff>
--- a/case_input_test_PGP_wind_solar.xlsx
+++ b/case_input_test_PGP_wind_solar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E8F37D5-7A2A-422B-BEB4-B20F4C9FF583}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F16483A-C782-4F27-991D-5BDFF53ACB29}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15500" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15495" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="100">
   <si>
     <t>This file is documentation for the input data format for the case definition file, used as input for the Simple Energy Model v 1.0</t>
   </si>
@@ -262,9 +262,6 @@
     <t>demand_series_Shaner_normalized_to_1_mean.csv</t>
   </si>
   <si>
-    <t>test_PGP</t>
-  </si>
-  <si>
     <t>CAPACITY_COST_PGP_STORAGE</t>
   </si>
   <si>
@@ -277,9 +274,6 @@
     <t>PGP_STORAGE_CHARGING_EFFICIENCY</t>
   </si>
   <si>
-    <t>1e-6 adds on about 1 cent per kWh if used one cycle per year</t>
-  </si>
-  <si>
     <t>($/h)/kW</t>
   </si>
   <si>
@@ -289,18 +283,6 @@
     <t>0.014 is default value</t>
   </si>
   <si>
-    <t>battery01</t>
-  </si>
-  <si>
-    <t>battery003</t>
-  </si>
-  <si>
-    <t>battery1</t>
-  </si>
-  <si>
-    <t>battery03</t>
-  </si>
-  <si>
     <t>QUICK_LOOK</t>
   </si>
   <si>
@@ -313,18 +295,9 @@
     <t>CAPACITY_COST_FROM_PGP_STORAGE</t>
   </si>
   <si>
-    <t xml:space="preserve">Electrolyser $1100 per kW capital cost. Assume 10% capital recovery factor and 10,000 hours per year = </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Electrolyser $4600 per kW capital cost. Assume 10% capital recovery factor and 10,000 hours per year = </t>
-  </si>
-  <si>
     <t>($/h)/kWh</t>
   </si>
   <si>
-    <t>If we assume $261/kWh capacity with a 10% cap recovery factor and 10,000 hours per year (and 6 hour charge/discharge time)</t>
-  </si>
-  <si>
     <t>from $1568/kW and $261/kWh from Davis et al 2018</t>
   </si>
   <si>
@@ -332,6 +305,21 @@
   </si>
   <si>
     <t>Nomalize demand 1.</t>
+  </si>
+  <si>
+    <t>If we assume $261/kWh capacity with a 8% cap recovery factor and 8760 hours per year (and 6 hour charge/discharge time)</t>
+  </si>
+  <si>
+    <t>2.7e-6 adds on about 2.4 cents per kWh if used one cycle per year</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Electrolyser $4600 per kW capital cost. Assume 8% capital recovery factor and 8760 hours per year = </t>
+  </si>
+  <si>
+    <t>base_PGP</t>
+  </si>
+  <si>
+    <t>base</t>
   </si>
 </sst>
 </file>
@@ -1223,185 +1211,185 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C46" sqref="C46"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B97" sqref="B97"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.08984375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.54296875" style="1"/>
+    <col min="1" max="1" width="36.140625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>20</v>
       </c>
@@ -1409,18 +1397,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>80</v>
+        <v>98</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
         <v>24</v>
       </c>
@@ -1431,12 +1419,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
         <v>27</v>
       </c>
@@ -1447,7 +1435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
         <v>29</v>
       </c>
@@ -1458,34 +1446,34 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B44" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C44" s="2" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="B46" s="12" t="b">
         <v>1</v>
       </c>
       <c r="C46" s="2" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
         <v>31</v>
       </c>
@@ -1496,7 +1484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -1507,7 +1495,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -1518,10 +1506,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>33</v>
       </c>
@@ -1530,10 +1518,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
         <v>35</v>
       </c>
@@ -1542,13 +1530,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
         <v>36</v>
       </c>
@@ -1558,7 +1546,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
         <v>37</v>
       </c>
@@ -1568,7 +1556,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A57" s="5" t="s">
         <v>38</v>
       </c>
@@ -1578,7 +1566,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A58" s="5" t="s">
         <v>39</v>
       </c>
@@ -1588,7 +1576,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A59" s="5" t="s">
         <v>40</v>
       </c>
@@ -1598,7 +1586,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A60" s="5" t="s">
         <v>41</v>
       </c>
@@ -1608,7 +1596,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A61" s="5" t="s">
         <v>42</v>
       </c>
@@ -1618,7 +1606,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A62" s="5" t="s">
         <v>43</v>
       </c>
@@ -1628,13 +1616,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A64" s="5" t="s">
         <v>44</v>
       </c>
@@ -1644,7 +1632,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A65" s="5" t="s">
         <v>45</v>
       </c>
@@ -1652,11 +1640,11 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C65" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>46</v>
       </c>
@@ -1669,13 +1657,13 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A68" s="5" t="s">
         <v>48</v>
       </c>
@@ -1685,7 +1673,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A69" s="5" t="s">
         <v>49</v>
       </c>
@@ -1693,11 +1681,11 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="C69" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -1709,13 +1697,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -1723,13 +1711,13 @@
         <v>-1</v>
       </c>
       <c r="C72" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D72" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="D72" s="2" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -1738,17 +1726,17 @@
         <v>2.3E-2</v>
       </c>
       <c r="C73" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
@@ -1756,13 +1744,13 @@
         <v>-1</v>
       </c>
       <c r="C75" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D75" s="2" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
@@ -1770,31 +1758,32 @@
         <v>1E-3</v>
       </c>
       <c r="C76" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A77" s="5"/>
       <c r="B77" s="12"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
       <c r="B78" s="12">
-        <v>2.6099999999999999E-3</v>
+        <f>261*0.08/8760</f>
+        <v>2.3835616438356165E-3</v>
       </c>
       <c r="C78" s="2" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
       <c r="D78" s="2" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -1802,11 +1791,11 @@
         <v>0</v>
       </c>
       <c r="C79" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -1814,11 +1803,11 @@
         <v>0</v>
       </c>
       <c r="C80" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -1828,7 +1817,7 @@
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -1846,7 +1835,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -1857,84 +1846,87 @@
         <v>64</v>
       </c>
       <c r="D83" s="2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A84" s="5"/>
       <c r="B84" s="12"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A85" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="B85" s="12">
+        <f>0.3*0.08/8760</f>
+        <v>2.7397260273972604E-6</v>
+      </c>
+      <c r="C85" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="D85" s="2" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A86" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B86" s="12">
+        <f>1100*0.08/8760</f>
+        <v>1.0045662100456621E-2</v>
+      </c>
+      <c r="C86" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D86" s="2" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A87" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="B87" s="12">
+        <f>4600*0.08/8760</f>
+        <v>4.2009132420091327E-2</v>
+      </c>
+      <c r="C87" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="D87" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A88" s="5" t="s">
         <v>81</v>
-      </c>
-      <c r="B85" s="12">
-        <v>9.9999999999999995E-7</v>
-      </c>
-      <c r="C85" s="2" t="s">
-        <v>99</v>
-      </c>
-      <c r="D85" s="2" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A86" s="5" t="s">
-        <v>95</v>
-      </c>
-      <c r="B86" s="12">
-        <v>1.0999999999999999E-2</v>
-      </c>
-      <c r="C86" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D86" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A87" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B87" s="12">
-        <v>4.5999999999999999E-2</v>
-      </c>
-      <c r="C87" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="D87" s="2" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
-      <c r="A88" s="5" t="s">
-        <v>82</v>
       </c>
       <c r="B88" s="12">
         <v>0</v>
       </c>
       <c r="C88" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A89" s="5" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B89" s="12">
         <v>0</v>
       </c>
       <c r="C89" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A90" s="5" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B90" s="12">
         <v>0.3</v>
@@ -1942,13 +1934,13 @@
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -1956,19 +1948,19 @@
         <v>10</v>
       </c>
       <c r="C92" s="2" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C94" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A95" s="3" t="s">
         <v>66</v>
       </c>
@@ -1977,57 +1969,30 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A96" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="B96" s="5" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A98" s="8" t="s">
-        <v>91</v>
-      </c>
-      <c r="B98" s="8">
-        <v>0.01</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A99" s="8" t="s">
-        <v>92</v>
-      </c>
-      <c r="B99" s="8">
-        <v>3.0000000000000001E-3</v>
-      </c>
-    </row>
-    <row r="100" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A100" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="B100" s="8">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="101" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A101" s="8" t="s">
-        <v>90</v>
-      </c>
-      <c r="B101" s="8">
-        <v>2.9999999999999997E-4</v>
-      </c>
-    </row>
-    <row r="103" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A103" s="3" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="B99" s="1"/>
+    </row>
+    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A100" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B103" s="11"/>
-    </row>
-    <row r="107" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A107" s="1" t="s">
+      <c r="B100" s="11"/>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A104" s="1" t="s">
         <v>70</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed problem with text to boolean translation
</commit_message>
<xml_diff>
--- a/case_input_test_PGP_wind_solar.xlsx
+++ b/case_input_test_PGP_wind_solar.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kcaldeira\Google Drive\git\SEM-1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F16483A-C782-4F27-991D-5BDFF53ACB29}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B91F99F-E2AC-48CC-8923-5B1F6CE649D3}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15495" windowHeight="7935" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15500" windowHeight="7940" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="case_input" sheetId="1" r:id="rId1"/>
@@ -316,10 +316,10 @@
     <t xml:space="preserve">Electrolyser $4600 per kW capital cost. Assume 8% capital recovery factor and 8760 hours per year = </t>
   </si>
   <si>
+    <t>base</t>
+  </si>
+  <si>
     <t>base_PGP</t>
-  </si>
-  <si>
-    <t>base</t>
   </si>
 </sst>
 </file>
@@ -1213,183 +1213,183 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F104"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B97" sqref="B97"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="F46" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="16.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="16.54296875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="36.140625" style="1" customWidth="1"/>
-    <col min="2" max="2" width="35.7109375" style="10" customWidth="1"/>
-    <col min="3" max="16384" width="16.5703125" style="1"/>
+    <col min="1" max="1" width="36.08984375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="35.7265625" style="10" customWidth="1"/>
+    <col min="3" max="16384" width="16.54296875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" s="7" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A1" s="7" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="9"/>
     </row>
-    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B2" s="10"/>
     </row>
-    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="10"/>
     </row>
-    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B4" s="10"/>
     </row>
-    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>2</v>
       </c>
       <c r="B5" s="10"/>
     </row>
-    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B6" s="10"/>
     </row>
-    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
       <c r="B7" s="10"/>
     </row>
-    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B8" s="10"/>
     </row>
-    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
       <c r="B9" s="10"/>
     </row>
-    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B10" s="10"/>
     </row>
-    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
         <v>6</v>
       </c>
       <c r="B11" s="10"/>
     </row>
-    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B12" s="10"/>
     </row>
-    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2" t="s">
         <v>7</v>
       </c>
       <c r="B13" s="10"/>
     </row>
-    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B14" s="10"/>
     </row>
-    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2" t="s">
         <v>8</v>
       </c>
       <c r="B15" s="10"/>
     </row>
-    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2" t="s">
         <v>9</v>
       </c>
       <c r="B16" s="10"/>
     </row>
-    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="10"/>
     </row>
-    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2" t="s">
         <v>10</v>
       </c>
       <c r="B18" s="10"/>
     </row>
-    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="10"/>
     </row>
-    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2" t="s">
         <v>11</v>
       </c>
       <c r="B20" s="10"/>
     </row>
-    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="10"/>
     </row>
-    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2" t="s">
         <v>12</v>
       </c>
       <c r="B22" s="10"/>
     </row>
-    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B23" s="10"/>
     </row>
-    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B24" s="10"/>
     </row>
-    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B25" s="10"/>
     </row>
-    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B26" s="10"/>
     </row>
-    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B27" s="10"/>
     </row>
-    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B28" s="10"/>
     </row>
-    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B29" s="10"/>
     </row>
-    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B30" s="10"/>
     </row>
-    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B31" s="10"/>
     </row>
-    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:2" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B32" s="10"/>
     </row>
-    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B33" s="10"/>
     </row>
-    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B34" s="10"/>
     </row>
-    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:3" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B35" s="10"/>
     </row>
-    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A37" s="3" t="s">
         <v>20</v>
       </c>
@@ -1397,18 +1397,18 @@
         <v>21</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A39" s="5" t="s">
         <v>22</v>
       </c>
       <c r="B39" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A40" s="5" t="s">
         <v>24</v>
       </c>
@@ -1419,12 +1419,12 @@
         <v>26</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A41" s="5"/>
       <c r="B41" s="12"/>
       <c r="C41" s="2"/>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A42" s="5" t="s">
         <v>27</v>
       </c>
@@ -1435,7 +1435,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A43" s="5" t="s">
         <v>29</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A44" s="5" t="s">
         <v>87</v>
       </c>
@@ -1457,12 +1457,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A45" s="5"/>
       <c r="B45" s="12"/>
       <c r="C45" s="2"/>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A46" s="5" t="s">
         <v>93</v>
       </c>
@@ -1473,7 +1473,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A47" s="5" t="s">
         <v>31</v>
       </c>
@@ -1484,7 +1484,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A48" s="5" t="s">
         <v>71</v>
       </c>
@@ -1495,7 +1495,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A49" s="5" t="s">
         <v>72</v>
       </c>
@@ -1506,10 +1506,10 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C50" s="2"/>
     </row>
-    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="3" t="s">
         <v>33</v>
       </c>
@@ -1518,10 +1518,10 @@
       </c>
       <c r="C51" s="4"/>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" x14ac:dyDescent="0.35">
       <c r="C52" s="2"/>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A53" s="5" t="s">
         <v>35</v>
       </c>
@@ -1530,13 +1530,13 @@
       </c>
       <c r="C53" s="2"/>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A54" s="5"/>
       <c r="B54" s="12"/>
       <c r="C54" s="2"/>
       <c r="D54" s="2"/>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A55" s="5" t="s">
         <v>36</v>
       </c>
@@ -1546,7 +1546,7 @@
       <c r="C55" s="2"/>
       <c r="D55" s="2"/>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A56" s="5" t="s">
         <v>37</v>
       </c>
@@ -1556,7 +1556,7 @@
       <c r="C56" s="2"/>
       <c r="D56" s="2"/>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A57" s="5" t="s">
         <v>38</v>
       </c>
@@ -1566,7 +1566,7 @@
       <c r="C57" s="2"/>
       <c r="D57" s="2"/>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A58" s="5" t="s">
         <v>39</v>
       </c>
@@ -1576,7 +1576,7 @@
       <c r="C58" s="2"/>
       <c r="D58" s="2"/>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A59" s="5" t="s">
         <v>40</v>
       </c>
@@ -1586,7 +1586,7 @@
       <c r="C59" s="2"/>
       <c r="D59" s="2"/>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A60" s="5" t="s">
         <v>41</v>
       </c>
@@ -1596,7 +1596,7 @@
       <c r="C60" s="2"/>
       <c r="D60" s="2"/>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A61" s="5" t="s">
         <v>42</v>
       </c>
@@ -1606,7 +1606,7 @@
       <c r="C61" s="2"/>
       <c r="D61" s="2"/>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A62" s="5" t="s">
         <v>43</v>
       </c>
@@ -1616,13 +1616,13 @@
       <c r="C62" s="2"/>
       <c r="D62" s="2"/>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A63" s="5"/>
       <c r="B63" s="12"/>
       <c r="C63" s="2"/>
       <c r="D63" s="2"/>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A64" s="5" t="s">
         <v>44</v>
       </c>
@@ -1632,7 +1632,7 @@
       <c r="C64" s="2"/>
       <c r="D64" s="2"/>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A65" s="5" t="s">
         <v>45</v>
       </c>
@@ -1644,7 +1644,7 @@
       </c>
       <c r="D65" s="2"/>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A66" s="5" t="s">
         <v>46</v>
       </c>
@@ -1657,13 +1657,13 @@
       </c>
       <c r="D66" s="2"/>
     </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A67" s="5"/>
       <c r="B67" s="12"/>
       <c r="C67" s="2"/>
       <c r="D67" s="2"/>
     </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A68" s="5" t="s">
         <v>48</v>
       </c>
@@ -1673,7 +1673,7 @@
       <c r="C68" s="2"/>
       <c r="D68" s="2"/>
     </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A69" s="5" t="s">
         <v>49</v>
       </c>
@@ -1685,7 +1685,7 @@
       </c>
       <c r="D69" s="2"/>
     </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A70" s="5" t="s">
         <v>50</v>
       </c>
@@ -1697,13 +1697,13 @@
       </c>
       <c r="D70" s="2"/>
     </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A71" s="5"/>
       <c r="B71" s="12"/>
       <c r="C71" s="2"/>
       <c r="D71" s="2"/>
     </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A72" s="5" t="s">
         <v>52</v>
       </c>
@@ -1717,7 +1717,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A73" s="5" t="s">
         <v>53</v>
       </c>
@@ -1730,13 +1730,13 @@
       </c>
       <c r="D73" s="2"/>
     </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A74" s="5"/>
       <c r="B74" s="12"/>
       <c r="C74" s="2"/>
       <c r="D74" s="2"/>
     </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A75" s="5" t="s">
         <v>54</v>
       </c>
@@ -1750,7 +1750,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A76" s="5" t="s">
         <v>55</v>
       </c>
@@ -1762,13 +1762,13 @@
       </c>
       <c r="D76" s="2"/>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A77" s="5"/>
       <c r="B77" s="12"/>
       <c r="C77" s="2"/>
       <c r="D77" s="2"/>
     </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A78" s="5" t="s">
         <v>56</v>
       </c>
@@ -1783,7 +1783,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A79" s="5" t="s">
         <v>57</v>
       </c>
@@ -1795,7 +1795,7 @@
       </c>
       <c r="D79" s="2"/>
     </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A80" s="5" t="s">
         <v>58</v>
       </c>
@@ -1807,7 +1807,7 @@
       </c>
       <c r="D80" s="2"/>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A81" s="5" t="s">
         <v>59</v>
       </c>
@@ -1817,7 +1817,7 @@
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
     </row>
-    <row r="82" spans="1:6" ht="12.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="13" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A82" s="5" t="s">
         <v>60</v>
       </c>
@@ -1835,7 +1835,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A83" s="5" t="s">
         <v>63</v>
       </c>
@@ -1849,13 +1849,13 @@
         <v>92</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A84" s="5"/>
       <c r="B84" s="12"/>
       <c r="C84" s="2"/>
       <c r="D84" s="2"/>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A85" s="5" t="s">
         <v>80</v>
       </c>
@@ -1870,7 +1870,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A86" s="5" t="s">
         <v>89</v>
       </c>
@@ -1885,7 +1885,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A87" s="5" t="s">
         <v>90</v>
       </c>
@@ -1900,7 +1900,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A88" s="5" t="s">
         <v>81</v>
       </c>
@@ -1912,7 +1912,7 @@
       </c>
       <c r="D88" s="2"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A89" s="5" t="s">
         <v>82</v>
       </c>
@@ -1924,7 +1924,7 @@
       </c>
       <c r="D89" s="2"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A90" s="5" t="s">
         <v>83</v>
       </c>
@@ -1934,13 +1934,13 @@
       <c r="C90" s="2"/>
       <c r="D90" s="2"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A91" s="5"/>
       <c r="B91" s="12"/>
       <c r="C91" s="2"/>
       <c r="D91" s="2"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="A92" s="5" t="s">
         <v>65</v>
       </c>
@@ -1952,15 +1952,15 @@
       </c>
       <c r="D92" s="2"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C93" s="2"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C94" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A95" s="3" t="s">
         <v>66</v>
       </c>
@@ -1969,29 +1969,29 @@
       </c>
       <c r="C95" s="4"/>
     </row>
-    <row r="96" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" s="5" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A96" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="97" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B97" s="1"/>
     </row>
-    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:2" s="6" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A98" s="8" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="99" spans="1:2" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.35">
       <c r="B99" s="1"/>
     </row>
-    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:2" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A100" s="3" t="s">
         <v>69</v>
       </c>
       <c r="B100" s="11"/>
     </row>
-    <row r="104" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A104" s="1" t="s">
         <v>70</v>
       </c>

</xml_diff>